<commit_message>
Formatted Round 11 Forecasts
</commit_message>
<xml_diff>
--- a/2016SuperRugby/Weekly Forecasts/Round_11.xlsx
+++ b/2016SuperRugby/Weekly Forecasts/Round_11.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RugbyPredictifier\RugbyPredictifier\2016SuperRugby\Weekly Forecasts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Friday" sheetId="1" r:id="rId1"/>
     <sheet name="Saturday" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Chance of Winning</t>
   </si>
@@ -134,12 +139,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#0%"/>
     <numFmt numFmtId="165" formatCode="#0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +421,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -462,7 +475,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,9 +507,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -528,6 +542,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -703,7 +718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -711,9 +726,15 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -736,7 +757,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -744,33 +765,33 @@
         <v>0.846082</v>
       </c>
       <c r="C2" s="6">
-        <v>0.137497</v>
+        <v>0.13749700000000001</v>
       </c>
       <c r="E2" s="6">
-        <v>0.554039</v>
+        <v>0.55403899999999995</v>
       </c>
       <c r="F2" s="6">
-        <v>0.4186196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:61">
+        <v>0.41861959999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>37.1969366</v>
+        <v>37.196936600000001</v>
       </c>
       <c r="C3" s="7">
-        <v>17.2115548</v>
+        <v>17.211554799999998</v>
       </c>
       <c r="E3" s="7">
-        <v>28.9470656</v>
+        <v>28.947065599999998</v>
       </c>
       <c r="F3" s="7">
-        <v>25.5967748</v>
-      </c>
-    </row>
-    <row r="4" spans="1:61">
+        <v>25.596774799999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -787,7 +808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -804,7 +825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -821,7 +842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -838,7 +859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -855,7 +876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -872,7 +893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -889,7 +910,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -906,7 +927,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -923,7 +944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -940,7 +961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -957,7 +978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -974,7 +995,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -991,7 +1012,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -1008,7 +1029,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1025,7 +1046,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1042,7 +1063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1059,7 +1080,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1076,7 +1097,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -1093,29 +1114,29 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="6">
-        <v>0.4828068</v>
+        <v>0.48280679999999998</v>
       </c>
       <c r="C23" s="6">
-        <v>0.014359</v>
+        <v>1.4359E-2</v>
       </c>
       <c r="E23" s="6">
         <v>0.209783</v>
       </c>
       <c r="F23" s="6">
-        <v>0.0920044</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>9.20044E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="6">
-        <v>0.0650386</v>
+        <v>6.5038600000000002E-2</v>
       </c>
       <c r="C24" s="6">
         <v>0.103244</v>
@@ -1124,7 +1145,7 @@
         <v>0.1314398</v>
       </c>
       <c r="F24" s="6">
-        <v>0.14027</v>
+        <v>0.14027000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1133,7 +1154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1141,9 +1162,21 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="B1" s="8" t="s">
         <v>28</v>
       </c>
@@ -1193,77 +1226,77 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>0.3969388</v>
+        <v>0.39693879999999998</v>
       </c>
       <c r="C2" s="6">
-        <v>0.5813194</v>
+        <v>0.58131940000000004</v>
       </c>
       <c r="E2" s="6">
-        <v>0.6182872</v>
+        <v>0.61828720000000004</v>
       </c>
       <c r="F2" s="6">
-        <v>0.3597004</v>
+        <v>0.35970039999999998</v>
       </c>
       <c r="H2" s="6">
-        <v>0.5789862</v>
+        <v>0.57898620000000001</v>
       </c>
       <c r="I2" s="6">
-        <v>0.3969216</v>
+        <v>0.39692159999999999</v>
       </c>
       <c r="K2" s="6">
-        <v>0.3246836</v>
+        <v>0.32468360000000002</v>
       </c>
       <c r="L2" s="6">
         <v>0.6434088</v>
       </c>
       <c r="N2" s="6">
-        <v>0.0643212</v>
+        <v>6.4321199999999995E-2</v>
       </c>
       <c r="O2" s="6">
         <v>0.9290872</v>
       </c>
     </row>
-    <row r="3" spans="1:61">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>31.8093476</v>
+        <v>31.809347599999999</v>
       </c>
       <c r="C3" s="7">
-        <v>36.9681192</v>
+        <v>36.968119199999997</v>
       </c>
       <c r="E3" s="7">
-        <v>33.5735106</v>
+        <v>33.573510599999999</v>
       </c>
       <c r="F3" s="7">
-        <v>26.9785472</v>
+        <v>26.978547200000001</v>
       </c>
       <c r="H3" s="7">
-        <v>32.9239054</v>
+        <v>32.923905400000002</v>
       </c>
       <c r="I3" s="7">
         <v>28.057661</v>
       </c>
       <c r="K3" s="7">
-        <v>17.2292306</v>
+        <v>17.229230600000001</v>
       </c>
       <c r="L3" s="7">
-        <v>23.855219</v>
+        <v>23.855219000000002</v>
       </c>
       <c r="N3" s="7">
         <v>20.494543</v>
       </c>
       <c r="O3" s="7">
-        <v>52.8372576</v>
-      </c>
-    </row>
-    <row r="4" spans="1:61">
+        <v>52.837257600000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1298,7 +1331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:61">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1333,7 +1366,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:61">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1368,7 +1401,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:61">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1403,7 +1436,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:61">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1438,7 +1471,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1473,7 +1506,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1508,7 +1541,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1543,7 +1576,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1578,7 +1611,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1613,7 +1646,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1648,7 +1681,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -1683,7 +1716,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1718,7 +1751,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -1753,7 +1786,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1788,7 +1821,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1823,7 +1856,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1858,7 +1891,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1893,7 +1926,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -1928,47 +1961,47 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="6">
-        <v>0.1418404</v>
+        <v>0.14184040000000001</v>
       </c>
       <c r="C23" s="6">
-        <v>0.207359</v>
+        <v>0.20735899999999999</v>
       </c>
       <c r="E23" s="6">
         <v>0.294796</v>
       </c>
       <c r="F23" s="6">
-        <v>0.0628172</v>
+        <v>6.2817200000000004E-2</v>
       </c>
       <c r="H23" s="6">
-        <v>0.2241858</v>
+        <v>0.22418579999999999</v>
       </c>
       <c r="I23" s="6">
         <v>0.1249914</v>
       </c>
       <c r="K23" s="6">
-        <v>0.0346516</v>
+        <v>3.4651599999999998E-2</v>
       </c>
       <c r="L23" s="6">
-        <v>0.2274684</v>
+        <v>0.22746839999999999</v>
       </c>
       <c r="N23" s="6">
-        <v>0.0085378</v>
+        <v>8.5377999999999999E-3</v>
       </c>
       <c r="O23" s="6">
-        <v>0.7064904</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+        <v>0.70649039999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="6">
-        <v>0.1255818</v>
+        <v>0.12558179999999999</v>
       </c>
       <c r="C24" s="6">
         <v>0.1164384</v>
@@ -1977,13 +2010,13 @@
         <v>0.1235696</v>
       </c>
       <c r="F24" s="6">
-        <v>0.1404298</v>
+        <v>0.14042979999999999</v>
       </c>
       <c r="H24" s="6">
-        <v>0.119902</v>
+        <v>0.11990199999999999</v>
       </c>
       <c r="I24" s="6">
-        <v>0.1302108</v>
+        <v>0.13021079999999999</v>
       </c>
       <c r="K24" s="6">
         <v>0.1681626</v>
@@ -1992,10 +2025,10 @@
         <v>0.1373566</v>
       </c>
       <c r="N24" s="6">
-        <v>0.0574214</v>
+        <v>5.7421399999999997E-2</v>
       </c>
       <c r="O24" s="6">
-        <v>0.033119</v>
+        <v>3.3119000000000003E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>